<commit_message>
feat(msexcel): set ContentLayer.INVISIBLE for invisible sheet (#1876)
* feat(msexcel): ignore invisible sheet

* DCO Remediation Commit for Qiefan Jiang <jiangqiefan@bytedance.com>

I, Qiefan Jiang <jiangqiefan@bytedance.com>, hereby add my Signed-off-by to this commit: ca391f4908f44f301de54a97057f0b809f5ce66c

Signed-off-by: Qiefan Jiang <jiangqiefan@bytedance.com>

* retain invisible sheet with ContentLayer.INVISIBLE

Signed-off-by: Qiefan Jiang <jiangqiefan@bytedance.com>

* update UT

Signed-off-by: Qiefan Jiang <jiangqiefan@bytedance.com>

* fix: use Optional for python3.9

Signed-off-by: Qiefan Jiang <jiangqiefan@bytedance.com>

* DCO Remediation Commit for Qiefan Jiang <jiangqiefan@bytedance.com>

I, Qiefan Jiang <jiangqiefan@bytedance.com>, hereby add my Signed-off-by to this commit: a34371a90e30589f7485f3d15ab09483d39a3c9f

Signed-off-by: Qiefan Jiang <jiangqiefan@bytedance.com>

---------

Signed-off-by: Qiefan Jiang <jiangqiefan@bytedance.com>
</commit_message>
<xml_diff>
--- a/tests/data/xlsx/test-01.xlsx
+++ b/tests/data/xlsx/test-01.xlsx
@@ -1,21 +1,22 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11110"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10211"/>
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/taa/Documents/projects/tmp/docling/tests/data/xlsx/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/bytedance/rag/opensource/docling/tests/data/xlsx/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{945BD0F7-0ADB-A64A-9800-FEAA0742FEEC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{24F23DF9-99BA-744A-982A-14EFF12372E1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="12660" yWindow="-19220" windowWidth="28040" windowHeight="17440" activeTab="2" xr2:uid="{7BFEBC09-E794-024E-92A5-4E4755531B02}"/>
+    <workbookView xWindow="0" yWindow="760" windowWidth="34560" windowHeight="21580" activeTab="2" xr2:uid="{7BFEBC09-E794-024E-92A5-4E4755531B02}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
     <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
     <sheet name="Sheet3" sheetId="3" r:id="rId3"/>
+    <sheet name="Sheet4" sheetId="4" state="hidden" r:id="rId4"/>
   </sheets>
   <calcPr calcId="181029"/>
   <extLst>
@@ -38,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="21" uniqueCount="10">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="22" uniqueCount="11">
   <si>
     <t xml:space="preserve">first </t>
   </si>
@@ -69,17 +70,28 @@
   <si>
     <t>first (f)</t>
   </si>
+  <si>
+    <t>header</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="2">
     <font>
       <sz val="12"/>
       <color theme="1"/>
-      <name val="Aptos Narrow"/>
+      <name val="等线"/>
       <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="9"/>
+      <name val="等线"/>
+      <family val="3"/>
+      <charset val="134"/>
       <scheme val="minor"/>
     </font>
   </fonts>
@@ -110,7 +122,7 @@
     </xf>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle name="常规" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -128,7 +140,7 @@
 <file path=xl/charts/chart1.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
   <c:date1904 val="0"/>
-  <c:lang val="en-US"/>
+  <c:lang val="zh-CN"/>
   <c:roundedCorners val="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
@@ -190,7 +202,7 @@
               <a:cs typeface="+mn-cs"/>
             </a:defRPr>
           </a:pPr>
-          <a:endParaRPr lang="en-US"/>
+          <a:endParaRPr lang="zh-CN"/>
         </a:p>
       </c:txPr>
     </c:title>
@@ -613,7 +625,7 @@
                   <a:cs typeface="+mn-cs"/>
                 </a:defRPr>
               </a:pPr>
-              <a:endParaRPr lang="en-US"/>
+              <a:endParaRPr lang="zh-CN"/>
             </a:p>
           </c:txPr>
         </c:title>
@@ -651,7 +663,7 @@
                 <a:cs typeface="+mn-cs"/>
               </a:defRPr>
             </a:pPr>
-            <a:endParaRPr lang="en-US"/>
+            <a:endParaRPr lang="zh-CN"/>
           </a:p>
         </c:txPr>
         <c:crossAx val="309818255"/>
@@ -713,7 +725,7 @@
                 <a:cs typeface="+mn-cs"/>
               </a:defRPr>
             </a:pPr>
-            <a:endParaRPr lang="en-US"/>
+            <a:endParaRPr lang="zh-CN"/>
           </a:p>
         </c:txPr>
         <c:crossAx val="1284139040"/>
@@ -755,7 +767,7 @@
               <a:cs typeface="+mn-cs"/>
             </a:defRPr>
           </a:pPr>
-          <a:endParaRPr lang="en-US"/>
+          <a:endParaRPr lang="zh-CN"/>
         </a:p>
       </c:txPr>
     </c:legend>
@@ -792,7 +804,7 @@
       <a:pPr>
         <a:defRPr/>
       </a:pPr>
-      <a:endParaRPr lang="en-US"/>
+      <a:endParaRPr lang="zh-CN"/>
     </a:p>
   </c:txPr>
   <c:printSettings>
@@ -806,7 +818,7 @@
 <file path=xl/charts/chart2.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
   <c:date1904 val="0"/>
-  <c:lang val="en-US"/>
+  <c:lang val="zh-CN"/>
   <c:roundedCorners val="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
@@ -868,7 +880,7 @@
               <a:cs typeface="+mn-cs"/>
             </a:defRPr>
           </a:pPr>
-          <a:endParaRPr lang="en-US"/>
+          <a:endParaRPr lang="zh-CN"/>
         </a:p>
       </c:txPr>
     </c:title>
@@ -1033,7 +1045,7 @@
                   <a:cs typeface="+mn-cs"/>
                 </a:defRPr>
               </a:pPr>
-              <a:endParaRPr lang="en-US"/>
+              <a:endParaRPr lang="zh-CN"/>
             </a:p>
           </c:txPr>
         </c:title>
@@ -1071,7 +1083,7 @@
                 <a:cs typeface="+mn-cs"/>
               </a:defRPr>
             </a:pPr>
-            <a:endParaRPr lang="en-US"/>
+            <a:endParaRPr lang="zh-CN"/>
           </a:p>
         </c:txPr>
         <c:crossAx val="280933119"/>
@@ -1153,7 +1165,7 @@
                   <a:cs typeface="+mn-cs"/>
                 </a:defRPr>
               </a:pPr>
-              <a:endParaRPr lang="en-US"/>
+              <a:endParaRPr lang="zh-CN"/>
             </a:p>
           </c:txPr>
         </c:title>
@@ -1185,7 +1197,7 @@
                 <a:cs typeface="+mn-cs"/>
               </a:defRPr>
             </a:pPr>
-            <a:endParaRPr lang="en-US"/>
+            <a:endParaRPr lang="zh-CN"/>
           </a:p>
         </c:txPr>
         <c:crossAx val="280908351"/>
@@ -1233,7 +1245,7 @@
       <a:pPr>
         <a:defRPr/>
       </a:pPr>
-      <a:endParaRPr lang="en-US"/>
+      <a:endParaRPr lang="zh-CN"/>
     </a:p>
   </c:txPr>
   <c:printSettings>
@@ -2483,7 +2495,7 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office 主题​​">
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
@@ -2805,9 +2817,9 @@
       <selection sqref="A1:C7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:3">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -2818,7 +2830,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:3">
       <c r="A2">
         <v>1</v>
       </c>
@@ -2829,7 +2841,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:3">
       <c r="A3">
         <v>2</v>
       </c>
@@ -2840,7 +2852,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:3">
       <c r="A4">
         <v>3</v>
       </c>
@@ -2851,7 +2863,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:3">
       <c r="A5">
         <v>4</v>
       </c>
@@ -2862,7 +2874,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:3">
       <c r="A6">
         <v>5</v>
       </c>
@@ -2873,7 +2885,7 @@
         <v>-3</v>
       </c>
     </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:3">
       <c r="A7">
         <v>6</v>
       </c>
@@ -2885,6 +2897,7 @@
       </c>
     </row>
   </sheetData>
+  <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
@@ -2897,9 +2910,9 @@
       <selection activeCell="N28" sqref="N28"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
   <sheetData>
-    <row r="1" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:9">
       <c r="A1" t="s">
         <v>3</v>
       </c>
@@ -2913,7 +2926,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="2" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:9">
       <c r="A2">
         <v>1</v>
       </c>
@@ -2927,7 +2940,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="3" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:9">
       <c r="A3">
         <v>2</v>
       </c>
@@ -2941,7 +2954,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="4" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:9">
       <c r="A4">
         <v>3</v>
       </c>
@@ -2955,7 +2968,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="5" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:9">
       <c r="A5">
         <v>4</v>
       </c>
@@ -2978,7 +2991,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="6" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:9">
       <c r="A6">
         <v>5</v>
       </c>
@@ -3001,7 +3014,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="7" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:9">
       <c r="A7">
         <v>6</v>
       </c>
@@ -3024,7 +3037,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="8" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:9">
       <c r="A8">
         <v>7</v>
       </c>
@@ -3047,7 +3060,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="9" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:9">
       <c r="A9">
         <v>8</v>
       </c>
@@ -3070,7 +3083,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="14" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:9">
       <c r="C14" t="s">
         <v>3</v>
       </c>
@@ -3081,7 +3094,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="15" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:9">
       <c r="C15">
         <v>1</v>
       </c>
@@ -3092,7 +3105,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="16" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:9">
       <c r="C16">
         <v>2</v>
       </c>
@@ -3103,7 +3116,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="17" spans="3:5" x14ac:dyDescent="0.2">
+    <row r="17" spans="3:5">
       <c r="C17">
         <v>3</v>
       </c>
@@ -3114,7 +3127,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="18" spans="3:5" x14ac:dyDescent="0.2">
+    <row r="18" spans="3:5">
       <c r="C18">
         <v>4</v>
       </c>
@@ -3126,6 +3139,7 @@
       </c>
     </row>
   </sheetData>
+  <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <drawing r:id="rId1"/>
 </worksheet>
@@ -3136,12 +3150,12 @@
   <dimension ref="A1:G13"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="K15" sqref="K15"/>
+      <selection activeCell="E28" sqref="E28"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:7">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -3150,7 +3164,7 @@
       </c>
       <c r="C1" s="1"/>
     </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:7">
       <c r="A2" s="1"/>
       <c r="B2" t="s">
         <v>1</v>
@@ -3159,7 +3173,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:7">
       <c r="A3">
         <v>1</v>
       </c>
@@ -3170,7 +3184,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:7">
       <c r="A4" s="1">
         <v>3</v>
       </c>
@@ -3181,7 +3195,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:7">
       <c r="A5" s="1"/>
       <c r="B5">
         <v>6</v>
@@ -3190,7 +3204,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:7">
       <c r="A6">
         <v>8</v>
       </c>
@@ -3199,7 +3213,7 @@
       </c>
       <c r="C6" s="1"/>
     </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:7">
       <c r="A7">
         <v>10</v>
       </c>
@@ -3213,7 +3227,7 @@
       </c>
       <c r="G7" s="1"/>
     </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:7">
       <c r="E8" s="1"/>
       <c r="F8" t="s">
         <v>1</v>
@@ -3222,7 +3236,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="9" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:7">
       <c r="E9">
         <v>1</v>
       </c>
@@ -3233,7 +3247,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="10" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:7">
       <c r="E10" s="1">
         <v>3</v>
       </c>
@@ -3244,7 +3258,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="11" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:7">
       <c r="E11" s="1"/>
       <c r="F11">
         <v>6</v>
@@ -3253,7 +3267,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="12" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:7">
       <c r="E12">
         <v>8</v>
       </c>
@@ -3262,7 +3276,7 @@
       </c>
       <c r="G12" s="1"/>
     </row>
-    <row r="13" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:7">
       <c r="E13">
         <v>10</v>
       </c>
@@ -3280,7 +3294,34 @@
     <mergeCell ref="E7:E8"/>
     <mergeCell ref="F7:G7"/>
   </mergeCells>
+  <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <drawing r:id="rId1"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4933F67A-3FE8-2F4D-BB74-9586CAFC801B}">
+  <dimension ref="A1:A2"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C11" sqref="C11"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
+  <sheetData>
+    <row r="1" spans="1:1">
+      <c r="A1" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="2" spans="1:1">
+      <c r="A2">
+        <v>1</v>
+      </c>
+    </row>
+  </sheetData>
+  <phoneticPr fontId="1" type="noConversion"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>